<commit_message>
Fix once again bugs
</commit_message>
<xml_diff>
--- a/docs/source/_static/structure/DBDAT_TEMPLATE.xlsx
+++ b/docs/source/_static/structure/DBDAT_TEMPLATE.xlsx
@@ -75368,31 +75368,31 @@
       <formula1>'ACC.ASST_LN_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="G4:G5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>'ACC.ASST_LN_'!$B$1:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.ASST_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.ASST_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.ASST_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.ASST_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.ASST_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.ASST_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.ASST_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.ASST_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.ASST_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -75405,7 +75405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -75426,6 +75426,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>C</t>
         </is>
       </c>
@@ -75438,10 +75443,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -75455,6 +75465,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>E</t>
         </is>
       </c>
@@ -75465,7 +75480,7 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -75477,7 +75492,7 @@
           <t>H</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>O</t>
         </is>
@@ -75945,37 +75960,37 @@
       <formula1>'ACC.SHR_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>'ACC.SHR_'!$B$1:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J5 L4:L5 N4:N5 P4:P5 R4:R5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.SHR_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="K4:K5 M4:M5 O4:O5 Q4:Q5 S4:S5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.SHR_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J5 L4:L5 N4:N5 P4:P5 R4:R5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.SHR_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="K4:K5 M4:M5 O4:O5 Q4:Q5 S4:S5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.SHR_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J5 L4:L5 N4:N5 P4:P5 R4:R5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.SHR_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="K4:K5 M4:M5 O4:O5 Q4:Q5 S4:S5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.SHR_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J5 L4:L5 N4:N5 P4:P5 R4:R5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.SHR_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="K4:K5 M4:M5 O4:O5 Q4:Q5 S4:S5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.SHR_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J5 L4:L5 N4:N5 P4:P5 R4:R5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.SHR_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="K4:K5 M4:M5 O4:O5 Q4:Q5 S4:S5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.SHR_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.SHR_'!$D$1:$D$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -75988,7 +76003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -76009,6 +76024,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>C</t>
         </is>
       </c>
@@ -76021,10 +76041,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -76038,6 +76063,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>E</t>
         </is>
       </c>
@@ -76048,7 +76078,7 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -76060,7 +76090,7 @@
           <t>H</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>O</t>
         </is>
@@ -80929,31 +80959,31 @@
       <formula1>'ACC.LBLTY_LN_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="G4:G5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>"True,False"</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$B$1:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H5 J4:J5 L4:L5 N4:N5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$B$1:$B$5</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$5</formula1>
     </dataValidation>
     <dataValidation sqref="I4:I5 K4:K5 M4:M5 O4:O5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>'ACC.LBLTY_LN_'!$C$1:$C$2</formula1>
+      <formula1>'ACC.LBLTY_LN_'!$D$1:$D$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -80966,7 +80996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -80987,6 +81017,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>C</t>
         </is>
       </c>
@@ -80999,10 +81034,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -81016,6 +81056,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>E</t>
         </is>
       </c>
@@ -81026,7 +81071,7 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -81038,7 +81083,7 @@
           <t>H</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>O</t>
         </is>

</xml_diff>

<commit_message>
Fix copy files after change in source code
</commit_message>
<xml_diff>
--- a/docs/source/_static/structure/DBDAT_TEMPLATE.xlsx
+++ b/docs/source/_static/structure/DBDAT_TEMPLATE.xlsx
@@ -13497,7 +13497,7 @@
       <c r="J4" s="19" t="n"/>
       <c r="K4" s="19" t="n"/>
       <c r="L4" s="16" t="n"/>
-      <c r="M4" s="19" t="n"/>
+      <c r="M4" s="15" t="n"/>
       <c r="N4" s="16" t="n"/>
       <c r="O4" s="16" t="n"/>
       <c r="P4" s="16" t="n"/>
@@ -13562,7 +13562,7 @@
       <c r="J5" s="19" t="n"/>
       <c r="K5" s="19" t="n"/>
       <c r="L5" s="16" t="n"/>
-      <c r="M5" s="19" t="n"/>
+      <c r="M5" s="15" t="n"/>
       <c r="N5" s="16" t="n"/>
       <c r="O5" s="16" t="n"/>
       <c r="P5" s="16" t="n"/>
@@ -77026,15 +77026,15 @@
     <col width="22.95" customWidth="1" min="8" max="8"/>
     <col width="22.95" customWidth="1" min="9" max="9"/>
     <col width="22.95" customWidth="1" min="10" max="10"/>
-    <col width="22.95" customWidth="1" min="11" max="11"/>
-    <col width="22.95" customWidth="1" min="12" max="12"/>
+    <col width="21.6" customWidth="1" min="11" max="11"/>
+    <col width="21.6" customWidth="1" min="12" max="12"/>
     <col width="32.40000000000001" customWidth="1" min="13" max="13"/>
     <col width="32.40000000000001" customWidth="1" min="14" max="14"/>
     <col width="31.05" customWidth="1" min="15" max="15"/>
-    <col width="32.40000000000001" customWidth="1" min="16" max="16"/>
+    <col width="31.05" customWidth="1" min="16" max="16"/>
     <col width="32.40000000000001" customWidth="1" min="17" max="17"/>
     <col width="24.3" customWidth="1" min="18" max="18"/>
-    <col width="32.40000000000001" customWidth="1" min="19" max="19"/>
+    <col width="31.05" customWidth="1" min="19" max="19"/>
     <col width="24.3" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
@@ -77150,12 +77150,12 @@
       </c>
       <c r="K3" s="7" t="inlineStr">
         <is>
-          <t>INSDAT_RPRTR_OF</t>
+          <t>ICDAT_RPRTR_OF</t>
         </is>
       </c>
       <c r="L3" s="7" t="inlineStr">
         <is>
-          <t>PENDAT_RPRTR_OF</t>
+          <t>PFDAT_RPRTR_OF</t>
         </is>
       </c>
       <c r="M3" s="13" t="inlineStr">
@@ -77170,14 +77170,14 @@
       </c>
       <c r="O3" s="13" t="inlineStr">
         <is>
+          <t>ICDAT_RPRTR_OF.STATUS</t>
+        </is>
+      </c>
+      <c r="P3" s="13" t="inlineStr">
+        <is>
           <t>IFDAT_RPRTR_OF.STATUS</t>
         </is>
       </c>
-      <c r="P3" s="13" t="inlineStr">
-        <is>
-          <t>INSDAT_RPRTR_OF.STATUS</t>
-        </is>
-      </c>
       <c r="Q3" s="13" t="inlineStr">
         <is>
           <t>MIRDAT_RPRTR_OF.STATUS</t>
@@ -77190,7 +77190,7 @@
       </c>
       <c r="S3" s="13" t="inlineStr">
         <is>
-          <t>PENDAT_RPRTR_OF.STATUS</t>
+          <t>PFDAT_RPRTR_OF.STATUS</t>
         </is>
       </c>
       <c r="T3" s="13" t="inlineStr">
@@ -83434,12 +83434,12 @@
       </c>
       <c r="I3" s="7" t="inlineStr">
         <is>
+          <t>CTY</t>
+        </is>
+      </c>
+      <c r="J3" s="7" t="inlineStr">
+        <is>
           <t>CTY_LTN</t>
-        </is>
-      </c>
-      <c r="J3" s="7" t="inlineStr">
-        <is>
-          <t>CTY</t>
         </is>
       </c>
       <c r="K3" s="7" t="inlineStr">

</xml_diff>